<commit_message>
added avg to the answers.txt
</commit_message>
<xml_diff>
--- a/assingment2_graphs.xlsx
+++ b/assingment2_graphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="No kvm cpu" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
     </textPr>
   </connection>
   <connection id="5" name="native-cpu" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jacek/Dysk Google/Studia/S3MGR/Cloud Computing/UB/assignment2/native-cpu.csv" thousands=" " tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/jacek/Dysk Google/Studia/S3MGR/Cloud Computing/UB/assignment2/native-cpu.csv" thousands=" " tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -94,7 +94,7 @@
     </textPr>
   </connection>
   <connection id="6" name="native-disk-random" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jacek/Dysk Google/Studia/S3MGR/Cloud Computing/UB/assignment2/native-disk-random.csv" decimal="," thousands=" " tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/jacek/Dysk Google/Studia/S3MGR/Cloud Computing/UB/assignment2/native-disk-random.csv" decimal="," thousands=" " tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -102,7 +102,7 @@
     </textPr>
   </connection>
   <connection id="7" name="native-fork" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jacek/Dysk Google/Studia/S3MGR/Cloud Computing/UB/assignment2/native-fork.csv" thousands=" " tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/jacek/Dysk Google/Studia/S3MGR/Cloud Computing/UB/assignment2/native-fork.csv" thousands=" " tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -110,7 +110,7 @@
     </textPr>
   </connection>
   <connection id="8" name="native-mem" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jacek/Dysk Google/Studia/S3MGR/Cloud Computing/UB/assignment2/native-mem.csv" thousands=" " tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/jacek/Dysk Google/Studia/S3MGR/Cloud Computing/UB/assignment2/native-mem.csv" thousands=" " tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -260,7 +260,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -650,11 +649,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2130297936"/>
-        <c:axId val="2131575664"/>
+        <c:axId val="2126099712"/>
+        <c:axId val="2126115856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2130297936"/>
+        <c:axId val="2126099712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,7 +699,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -767,12 +765,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131575664"/>
+        <c:crossAx val="2126115856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2131575664"/>
+        <c:axId val="2126115856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +816,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -884,7 +881,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130297936"/>
+        <c:crossAx val="2126099712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1363,11 +1360,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2133344672"/>
-        <c:axId val="2133350640"/>
+        <c:axId val="2125733888"/>
+        <c:axId val="2125727920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2133344672"/>
+        <c:axId val="2125733888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,12 +1476,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133350640"/>
+        <c:crossAx val="2125727920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2133350640"/>
+        <c:axId val="2125727920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,7 +1601,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133344672"/>
+        <c:crossAx val="2125733888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1688,7 +1685,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>No KVM memory benchmark</a:t>
+              <a:t>KVM memory benchmark</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2083,11 +2080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2133396752"/>
-        <c:axId val="2133402720"/>
+        <c:axId val="2124579216"/>
+        <c:axId val="2124573248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2133396752"/>
+        <c:axId val="2124579216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2199,12 +2196,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133402720"/>
+        <c:crossAx val="2124573248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2133402720"/>
+        <c:axId val="2124573248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2324,7 +2321,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133396752"/>
+        <c:crossAx val="2124579216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2803,11 +2800,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2056682624"/>
-        <c:axId val="-2056495984"/>
+        <c:axId val="2125795536"/>
+        <c:axId val="2125801632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2056682624"/>
+        <c:axId val="2125795536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2919,12 +2916,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056495984"/>
+        <c:crossAx val="2125801632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2056495984"/>
+        <c:axId val="2125801632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3044,7 +3041,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056682624"/>
+        <c:crossAx val="2125795536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3133,7 +3130,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3523,11 +3519,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2130344608"/>
-        <c:axId val="2130350576"/>
+        <c:axId val="2126260304"/>
+        <c:axId val="2126266272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2130344608"/>
+        <c:axId val="2126260304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3573,7 +3569,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3639,12 +3634,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130350576"/>
+        <c:crossAx val="2126266272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2130350576"/>
+        <c:axId val="2126266272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3690,7 +3685,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3756,7 +3750,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130344608"/>
+        <c:crossAx val="2126260304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3853,7 +3847,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4243,11 +4236,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2022593024"/>
-        <c:axId val="-2020371856"/>
+        <c:axId val="2126313360"/>
+        <c:axId val="2126319328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2022593024"/>
+        <c:axId val="2126313360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4293,7 +4286,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4359,12 +4351,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2020371856"/>
+        <c:crossAx val="2126319328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2020371856"/>
+        <c:axId val="2126319328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4410,7 +4402,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4477,7 +4468,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2022593024"/>
+        <c:crossAx val="2126313360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4961,11 +4952,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2131713072"/>
-        <c:axId val="2131719056"/>
+        <c:axId val="2126363440"/>
+        <c:axId val="2126369424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2131713072"/>
+        <c:axId val="2126363440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5078,12 +5069,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131719056"/>
+        <c:crossAx val="2126369424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2131719056"/>
+        <c:axId val="2126369424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5140,7 +5131,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131713072"/>
+        <c:crossAx val="2126363440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5624,11 +5615,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2131730800"/>
-        <c:axId val="2131736784"/>
+        <c:axId val="2126413536"/>
+        <c:axId val="2126419520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2131730800"/>
+        <c:axId val="2126413536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5741,12 +5732,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131736784"/>
+        <c:crossAx val="2126419520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2131736784"/>
+        <c:axId val="2126419520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5803,7 +5794,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131730800"/>
+        <c:crossAx val="2126413536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5897,7 +5888,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6287,11 +6277,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2047329968"/>
-        <c:axId val="-2047260192"/>
+        <c:axId val="2126464736"/>
+        <c:axId val="2126470720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2047329968"/>
+        <c:axId val="2126464736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6337,7 +6327,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6404,12 +6393,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2047260192"/>
+        <c:crossAx val="2126470720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2047260192"/>
+        <c:axId val="2126470720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6466,7 +6455,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2047329968"/>
+        <c:crossAx val="2126464736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6555,7 +6544,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6945,11 +6933,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2131942704"/>
-        <c:axId val="2131936736"/>
+        <c:axId val="2125887248"/>
+        <c:axId val="2125881280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2131942704"/>
+        <c:axId val="2125887248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6995,7 +6983,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7061,12 +7048,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131936736"/>
+        <c:crossAx val="2125881280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2131936736"/>
+        <c:axId val="2125881280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7112,7 +7099,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7179,7 +7165,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131942704"/>
+        <c:crossAx val="2125887248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7268,7 +7254,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7658,11 +7643,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2131978736"/>
-        <c:axId val="2133254784"/>
+        <c:axId val="2125838320"/>
+        <c:axId val="2125832352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2131978736"/>
+        <c:axId val="2125838320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7708,7 +7693,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7774,12 +7758,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133254784"/>
+        <c:crossAx val="2125832352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2133254784"/>
+        <c:axId val="2125832352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7825,7 +7809,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7892,7 +7875,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131978736"/>
+        <c:crossAx val="2125838320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8371,11 +8354,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2031704672"/>
-        <c:axId val="-2031701728"/>
+        <c:axId val="2125786464"/>
+        <c:axId val="2125780496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2031704672"/>
+        <c:axId val="2125786464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8487,12 +8470,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2031701728"/>
+        <c:crossAx val="2125780496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2031701728"/>
+        <c:axId val="2125780496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8605,7 +8588,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2031704672"/>
+        <c:crossAx val="2125786464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17319,8 +17302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E3"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17940,7 +17923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>

</xml_diff>